<commit_message>
fix(OpportunityDataMapping): Fixed Issue with the VAT & Contact Mapping
* Resolved Correct Vat Type on Import

* Mapped `Contact Type` to `Contact` on Import
</commit_message>
<xml_diff>
--- a/tests/Feature/Data/opportunity/contacts-23032022.xlsx
+++ b/tests/Feature/Data/opportunity/contacts-23032022.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>Software</t>
   </si>
 </sst>
 </file>
@@ -178,7 +181,6 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <color indexed="64"/>
       <sz val="9.000000"/>
     </font>
   </fonts>
@@ -975,10 +977,81 @@
         <v>44</v>
       </c>
     </row>
+    <row r="4" ht="63.75">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>